<commit_message>
Lastet inn flere datasett i onto
</commit_message>
<xml_diff>
--- a/Datasett/Avfallspunkter.xlsx
+++ b/Datasett/Avfallspunkter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malin\Documents\Project_Y\Datasett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3C7361-F890-454B-857C-7F91484027B9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE39D58-7174-4D1B-842F-F69B373958AE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="91">
   <si>
     <t>kind</t>
   </si>
@@ -196,9 +196,6 @@
     <t>5.981664</t>
   </si>
   <si>
-    <t>X FV286 / Nevland</t>
-  </si>
-  <si>
     <t>Likker i krysset ved FV286 og veien opp til Nevland</t>
   </si>
   <si>
@@ -290,6 +287,12 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Giljastølen Camping</t>
+  </si>
+  <si>
+    <t>Nevland</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1136,13 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="35" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1167,10 +1173,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
         <v>88</v>
-      </c>
-      <c r="K1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1242,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -1509,13 +1515,13 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
       </c>
       <c r="H13">
         <v>4330</v>
@@ -1524,10 +1530,10 @@
         <v>50</v>
       </c>
       <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
         <v>61</v>
-      </c>
-      <c r="K13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1541,13 +1547,13 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>65</v>
       </c>
       <c r="H14">
         <v>4335</v>
@@ -1556,10 +1562,10 @@
         <v>13</v>
       </c>
       <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
         <v>66</v>
-      </c>
-      <c r="K14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1576,10 +1582,10 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" t="s">
         <v>68</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
       </c>
       <c r="H15">
         <v>4335</v>
@@ -1588,10 +1594,10 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
         <v>70</v>
-      </c>
-      <c r="K15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1605,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
         <v>72</v>
       </c>
-      <c r="E16" t="s">
-        <v>73</v>
-      </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16">
         <v>4335</v>
@@ -1620,10 +1626,10 @@
         <v>13</v>
       </c>
       <c r="J16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" t="s">
         <v>74</v>
-      </c>
-      <c r="K16" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1637,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="E17" t="s">
-        <v>77</v>
-      </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17">
         <v>4335</v>
@@ -1652,10 +1658,10 @@
         <v>13</v>
       </c>
       <c r="J17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
         <v>78</v>
-      </c>
-      <c r="K17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1669,13 +1675,13 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
         <v>80</v>
       </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18">
         <v>4335</v>
@@ -1684,10 +1690,10 @@
         <v>13</v>
       </c>
       <c r="J18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" t="s">
         <v>82</v>
-      </c>
-      <c r="K18" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1701,13 +1707,13 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
-        <v>85</v>
-      </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19">
         <v>4335</v>
@@ -1716,10 +1722,10 @@
         <v>13</v>
       </c>
       <c r="J19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K19" t="s">
         <v>86</v>
-      </c>
-      <c r="K19" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>